<commit_message>
3 tables finally done
</commit_message>
<xml_diff>
--- a/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_VVDM.xlsx
+++ b/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_VVDM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="185">
   <si>
     <t xml:space="preserve">pdf_page_number</t>
   </si>
@@ -227,6 +227,9 @@
     <t xml:space="preserve">ashei</t>
   </si>
   <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">sand</t>
   </si>
   <si>
@@ -272,9 +275,6 @@
     <t xml:space="preserve">90+</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
     <t xml:space="preserve">7-75</t>
   </si>
   <si>
@@ -420,6 +420,162 @@
   </si>
   <si>
     <t xml:space="preserve">70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kochia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prostrata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No storage, i.e. freshly collected seeds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage at 20degC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage at 2degC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage at -5degC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">646</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decidua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moist paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily light period during germination was 8 to 16 hours/Constant germination temperatures at 26 °C and at 20 °C also were used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moist paper or blotters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily light period during germination was 8 to 16 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gmelinii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moist paper/sand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kaempferi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily light period during germination was 8 to 16 hours/Constant germination temperatures at 24 °C and at 20 °C also were used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laricina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lyallii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USP 3% H2O2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occidentalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">104</t>
   </si>
 </sst>
 </file>
@@ -503,7 +659,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -530,6 +686,10 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1059,10 +1219,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE14"/>
+  <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE13" activeCellId="0" sqref="AE13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE35" activeCellId="0" sqref="AE35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1180,11 +1340,23 @@
       <c r="D2" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>68</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K2" s="3" t="n">
         <v>0</v>
@@ -1195,26 +1367,59 @@
       <c r="M2" s="3" t="n">
         <v>120</v>
       </c>
+      <c r="N2" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O2" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="W2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>70</v>
+      <c r="X2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,11 +1435,23 @@
       <c r="D3" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>68</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K3" s="3" t="n">
         <v>0</v>
@@ -1245,26 +1462,59 @@
       <c r="M3" s="3" t="n">
         <v>120</v>
       </c>
+      <c r="N3" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O3" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="S3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE3" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1278,43 +1528,88 @@
         <v>66</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L4" s="3" t="n">
         <v>5</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>84</v>
       </c>
+      <c r="U4" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="V4" s="5" t="s">
         <v>85</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,11 +1625,23 @@
       <c r="D5" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F5" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K5" s="3" t="n">
         <v>0</v>
@@ -1345,26 +1652,59 @@
       <c r="M5" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="N5" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O5" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="T5" s="5" t="s">
         <v>88</v>
       </c>
+      <c r="U5" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="V5" s="5" t="s">
         <v>89</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,11 +1720,23 @@
       <c r="D6" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="E6" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F6" s="5" t="s">
         <v>90</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="J6" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K6" s="3" t="n">
         <v>0</v>
@@ -1395,26 +1747,59 @@
       <c r="M6" s="3" t="s">
         <v>91</v>
       </c>
+      <c r="N6" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O6" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="U6" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="V6" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,11 +1815,23 @@
       <c r="D7" s="3" t="s">
         <v>93</v>
       </c>
+      <c r="E7" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F7" s="5" t="s">
         <v>94</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="J7" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K7" s="3" t="n">
         <v>0</v>
@@ -1445,26 +1842,59 @@
       <c r="M7" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="N7" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O7" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="T7" s="5" t="s">
         <v>95</v>
       </c>
+      <c r="U7" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="V7" s="5" t="s">
         <v>96</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1480,11 +1910,23 @@
       <c r="D8" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="E8" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F8" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="J8" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K8" s="3" t="n">
         <v>120</v>
@@ -1495,26 +1937,59 @@
       <c r="M8" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="N8" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O8" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="T8" s="5" t="s">
         <v>100</v>
       </c>
+      <c r="U8" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="V8" s="5" t="s">
         <v>101</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="AE8" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,17 +2005,23 @@
       <c r="D9" s="3" t="s">
         <v>102</v>
       </c>
+      <c r="E9" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F9" s="5" t="s">
         <v>103</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="H9" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="I9" s="3" t="s">
         <v>104</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K9" s="3" t="n">
         <v>0</v>
@@ -1551,26 +2032,59 @@
       <c r="M9" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="N9" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O9" s="3" t="s">
         <v>105</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>105</v>
       </c>
+      <c r="Q9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="S9" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="T9" s="5" t="s">
         <v>106</v>
       </c>
+      <c r="U9" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="V9" s="5" t="s">
         <v>107</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD9" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="AE9" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,17 +2100,23 @@
       <c r="D10" s="6" t="s">
         <v>102</v>
       </c>
+      <c r="E10" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F10" s="5" t="s">
         <v>103</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="H10" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="I10" s="3" t="s">
         <v>104</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K10" s="3" t="n">
         <v>30</v>
@@ -1607,26 +2127,59 @@
       <c r="M10" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="N10" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O10" s="3" t="s">
         <v>105</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>105</v>
       </c>
+      <c r="Q10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="S10" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>109</v>
       </c>
+      <c r="U10" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="V10" s="5" t="s">
         <v>107</v>
       </c>
       <c r="W10" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD10" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="AE10" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1642,11 +2195,23 @@
       <c r="D11" s="3" t="s">
         <v>110</v>
       </c>
+      <c r="E11" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F11" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K11" s="3" t="n">
         <v>120</v>
@@ -1657,11 +2222,20 @@
       <c r="M11" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="N11" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O11" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="S11" s="5" t="s">
         <v>111</v>
@@ -1669,14 +2243,38 @@
       <c r="T11" s="5" t="s">
         <v>112</v>
       </c>
+      <c r="U11" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="V11" s="5" t="s">
         <v>113</v>
       </c>
       <c r="W11" s="5" t="s">
         <v>114</v>
       </c>
+      <c r="X11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="AE11" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,11 +2290,23 @@
       <c r="D12" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="E12" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F12" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K12" s="3" t="n">
         <v>0</v>
@@ -1707,26 +2317,59 @@
       <c r="M12" s="3" t="s">
         <v>116</v>
       </c>
+      <c r="N12" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O12" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>117</v>
       </c>
+      <c r="Q12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="S12" s="5" t="s">
         <v>118</v>
       </c>
       <c r="T12" s="5" t="s">
         <v>119</v>
       </c>
+      <c r="U12" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="V12" s="5" t="s">
         <v>120</v>
       </c>
       <c r="W12" s="5" t="s">
         <v>121</v>
       </c>
+      <c r="X12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="AE12" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,17 +2385,23 @@
       <c r="D13" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="E13" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F13" s="5" t="s">
         <v>103</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>122</v>
       </c>
+      <c r="H13" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="I13" s="3" t="s">
         <v>123</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K13" s="3" t="n">
         <v>4</v>
@@ -1763,23 +2412,56 @@
       <c r="M13" s="3" t="s">
         <v>124</v>
       </c>
+      <c r="N13" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O13" s="3" t="s">
         <v>125</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>125</v>
       </c>
+      <c r="Q13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="S13" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T13" s="5" t="s">
         <v>126</v>
       </c>
+      <c r="U13" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="V13" s="5" t="s">
         <v>96</v>
       </c>
       <c r="W13" s="5" t="s">
         <v>127</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD13" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="AE13" s="3" t="s">
         <v>128</v>
@@ -1798,11 +2480,23 @@
       <c r="D14" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="E14" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F14" s="5" t="s">
         <v>129</v>
       </c>
+      <c r="G14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="J14" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K14" s="3" t="n">
         <v>0</v>
@@ -1813,26 +2507,3054 @@
       <c r="M14" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="N14" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="O14" s="3" t="s">
         <v>105</v>
       </c>
       <c r="P14" s="3" t="s">
         <v>105</v>
       </c>
+      <c r="Q14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="S14" s="5" t="s">
         <v>130</v>
       </c>
       <c r="T14" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="U14" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="V14" s="5" t="s">
         <v>89</v>
       </c>
       <c r="W14" s="5" t="s">
         <v>132</v>
       </c>
+      <c r="X14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="AE14" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD15" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE15" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE16" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE17" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD18" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE18" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD19" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE19" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD20" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD21" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD22" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD23" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD24" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD25" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD27" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD28" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD29" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD30" s="3" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD31" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD32" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD33" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34" s="7" t="n">
+        <v>1051200</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD34" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O35" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P35" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q35" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R35" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="S35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U35" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="V35" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="W35" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="X35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE35" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R36" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="S36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="V36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="X36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE36" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P37" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R37" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="S37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U37" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="V37" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="W37" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="X37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE37" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P38" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R38" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U38" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="V38" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="W38" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="X38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE38" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P39" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R39" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="S39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="V39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="X39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE39" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R40" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U40" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="V40" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="W40" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="X40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE40" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P41" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R41" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="S41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="V41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="X41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE41" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R42" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="S42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U42" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="V42" s="5" t="s">
         <v>75</v>
+      </c>
+      <c r="W42" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="X42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE42" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="P43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R43" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="S43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U43" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="V43" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="W43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="X43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE43" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R44" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U44" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="V44" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="W44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="X44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE44" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P45" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R45" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="S45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="V45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="X45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE45" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O46" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P46" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q46" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R46" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U46" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="V46" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W46" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="X46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE46" s="3" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>